<commit_message>
all api functions ok
</commit_message>
<xml_diff>
--- a/design/root.xlsx
+++ b/design/root.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\success-2025\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F267A345-0D88-43AE-AC0C-9A68D82AAAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD20EA21-C356-44A0-83D4-0EF294812489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
   <si>
     <t>/signup</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>/:userId/successList</t>
+  </si>
+  <si>
+    <t>Success güncelleme</t>
+  </si>
+  <si>
+    <t>Success silme</t>
   </si>
 </sst>
 </file>
@@ -265,13 +271,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -282,29 +285,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -586,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G21"/>
+  <dimension ref="B2:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,319 +600,349 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="3" t="str">
-        <f>CONCATENATE($B$2,C2)</f>
+      <c r="D2" s="2" t="str">
+        <f t="shared" ref="D2:D14" si="0">CONCATENATE($B$2,C2)</f>
         <v>/api/v1/users/:id</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>/api/v1/users/:userId/successList</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="8"/>
+      <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="3" t="str">
-        <f>CONCATENATE($B$2,C3)</f>
+      <c r="D4" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>/api/v1/users/signup</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G4" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="3" t="s">
+    <row r="5" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="8"/>
+      <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="str">
-        <f>CONCATENATE($B$2,C4)</f>
+      <c r="D5" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>/api/v1/users/login</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G5" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="3" t="s">
+    <row r="6" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="3" t="str">
-        <f>CONCATENATE($B$2,C5)</f>
+      <c r="D6" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>/api/v1/users/logout</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G6" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="3" t="str">
-        <f>CONCATENATE($B$2,C6)</f>
-        <v>/api/v1/users/:userId/successList</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
+    <row r="7" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>/api/v1/users/me</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="4" t="str">
-        <f>CONCATENATE($B$2,C7)</f>
-        <v>/api/v1/users/me</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="G7" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>/api/v1/users/updateMyPassword</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>/api/v1/users/updateMe</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>/api/v1/users/deleteMe</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>/api/v1/users/allUsers</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="4" t="str">
-        <f>CONCATENATE($B$2,C8)</f>
-        <v>/api/v1/users/updateMyPassword</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="G11" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>/api/v1/users/restrict/:id</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>/api/v1/users/restrict/:id</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="4" t="str">
-        <f>CONCATENATE($B$2,C9)</f>
-        <v>/api/v1/users/updateMe</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="4" t="str">
-        <f>CONCATENATE($B$2,C10)</f>
-        <v>/api/v1/users/deleteMe</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="4" t="s">
+      <c r="G13" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="8"/>
+      <c r="C14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>/api/v1/users/restrict/:id</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="5" t="str">
-        <f>CONCATENATE($B$2,C11)</f>
-        <v>/api/v1/users/allUsers</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="5" t="str">
-        <f>CONCATENATE($B$2,C12)</f>
-        <v>/api/v1/users/restrict/:id</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <f>CONCATENATE($B$2,C13)</f>
-        <v>/api/v1/users/restrict/:id</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="5" t="str">
-        <f>CONCATENATE($B$2,C14)</f>
-        <v>/api/v1/users/restrict/:id</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="2:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="11"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="18" spans="2:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="3" t="str">
+      <c r="D18" s="2" t="str">
         <f>CONCATENATE($B$18,C18)</f>
         <v>/api/v1/successes/</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3" t="s">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="3" t="s">
+      <c r="B19" s="10"/>
+      <c r="C19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="3" t="str">
+      <c r="D19" s="2" t="str">
         <f>CONCATENATE($B$18,C19)</f>
         <v>/api/v1/successes/:id</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3" t="s">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="5" t="s">
+      <c r="B20" s="10"/>
+      <c r="C20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="5" t="str">
+      <c r="D20" s="4" t="str">
         <f>CONCATENATE($B$18,C20)</f>
         <v>/api/v1/successes/</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="13"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="4" t="str">
+        <f>CONCATENATE($B$18,C21)</f>
+        <v>/api/v1/successes/:id</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="10"/>
+      <c r="C22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="4" t="str">
+        <f>CONCATENATE($B$18,C22)</f>
+        <v>/api/v1/successes/:id</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:B15"/>
-    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B18:B22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>